<commit_message>
fix bug of wrap nft
</commit_message>
<xml_diff>
--- a/files/nft_image_archive.xlsx
+++ b/files/nft_image_archive.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="24220"/>
+    <workbookView windowHeight="24160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="369">
   <si>
     <t>Canister</t>
   </si>
@@ -40,6 +40,9 @@
     <t>file type</t>
   </si>
   <si>
+    <t>storage canister</t>
+  </si>
+  <si>
     <t>bkvll-jiaaa-aaaah-qcqnq-cai</t>
   </si>
   <si>
@@ -1037,6 +1040,84 @@
   </si>
   <si>
     <t>https://xzxhy-oiaaa-aaaah-qclnq-cai.raw.ic0.app/?type=thumbnail&amp;tokenid=%s</t>
+  </si>
+  <si>
+    <t>jmuqr-yqaaa-aaaaj-qaicq-cai</t>
+  </si>
+  <si>
+    <t>ICP Squad</t>
+  </si>
+  <si>
+    <t>https://jmuqr-yqaaa-aaaaj-qaicq-cai.raw.ic0.app/?type=thumbnail&amp;tokenid=%s</t>
+  </si>
+  <si>
+    <t>2tvxo-eqaaa-aaaai-acjla-cai</t>
+  </si>
+  <si>
+    <t>IC Dream Whale</t>
+  </si>
+  <si>
+    <t>https://2tvxo-eqaaa-aaaai-acjla-cai.raw.ic0.app/?type=thumbnail&amp;tokenid=%s</t>
+  </si>
+  <si>
+    <t>png</t>
+  </si>
+  <si>
+    <t>x4oqm-bqaaa-aaaam-qahaq-cai</t>
+  </si>
+  <si>
+    <t>DRIP BANG</t>
+  </si>
+  <si>
+    <t>https://x4oqm-bqaaa-aaaam-qahaq-cai.raw.ic0.app/?type=thumbnail&amp;tokenid=%s</t>
+  </si>
+  <si>
+    <t>y5prr-fiaaa-aaaam-qagga-cai</t>
+  </si>
+  <si>
+    <t>DogFinity</t>
+  </si>
+  <si>
+    <t>https://y5prr-fiaaa-aaaam-qagga-cai.raw.ic0.app/?type=thumbnail&amp;tokenid=%s</t>
+  </si>
+  <si>
+    <t>6wghg-7yaaa-aaaam-qagra-cai</t>
+  </si>
+  <si>
+    <t>IC Baboons</t>
+  </si>
+  <si>
+    <t>https://6wghg-7yaaa-aaaam-qagra-cai.raw.ic0.app/?type=thumbnail&amp;tokenid=%s</t>
+  </si>
+  <si>
+    <t>jpeg</t>
+  </si>
+  <si>
+    <t>6eaq7-tiaaa-aaaam-qagsa-cai</t>
+  </si>
+  <si>
+    <t>DfinityPigs</t>
+  </si>
+  <si>
+    <t>https://6eaq7-tiaaa-aaaam-qagsa-cai.raw.ic0.app/?type=thumbnail&amp;tokenid=%s</t>
+  </si>
+  <si>
+    <t>vcpye-qyaaa-aaaak-qafjq-cai</t>
+  </si>
+  <si>
+    <t>Starfish</t>
+  </si>
+  <si>
+    <t>https://vcpye-qyaaa-aaaak-qafjq-cai.raw.ic0.app/?type=thumbnail&amp;tokenid=%s</t>
+  </si>
+  <si>
+    <t>tvo7m-iyaaa-aaaai-qjjsa-cai</t>
+  </si>
+  <si>
+    <t>IC Dinos Items</t>
+  </si>
+  <si>
+    <t>https://tvo7m-iyaaa-aaaai-qjjsa-cai.raw.ic0.app/?type=thumbnail&amp;tokenid=%s</t>
   </si>
   <si>
     <t>fp7fo-2aaaa</t>
@@ -1047,14 +1128,21 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -1106,6 +1194,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
@@ -1113,11 +1216,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1137,9 +1240,38 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1160,55 +1292,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1245,25 +1333,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1281,7 +1363,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1293,13 +1381,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1311,7 +1417,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1323,25 +1483,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1353,67 +1495,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1432,21 +1520,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1490,26 +1563,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1524,167 +1577,211 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="41">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="41">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1693,7 +1790,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2013,12 +2113,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:N149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A95" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.64285714285714" defaultRowHeight="17.6"/>
@@ -2029,2230 +2129,2434 @@
     <col min="4" max="4" width="11.3125" customWidth="1"/>
     <col min="5" max="5" width="13.2410714285714" customWidth="1"/>
     <col min="6" max="6" width="48.3660714285714" customWidth="1"/>
-    <col min="7" max="7" width="33.3303571428571" style="2" customWidth="1"/>
+    <col min="7" max="7" width="33.3303571428571" style="4" customWidth="1"/>
     <col min="8" max="8" width="15.9196428571429" customWidth="1"/>
+    <col min="9" max="9" width="27.0803571428571" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1" spans="1:8">
-      <c r="A1" t="s">
+    <row r="1" customFormat="1" spans="1:9">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="1" spans="1:8">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="2">
+        <v>12</v>
+      </c>
+      <c r="G2" s="4">
         <v>1000</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="1" spans="1:8">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="2">
+        <v>12</v>
+      </c>
+      <c r="G3" s="4">
         <v>69</v>
       </c>
       <c r="H3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="1" spans="1:8">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="2">
+        <v>12</v>
+      </c>
+      <c r="G4" s="4">
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:8">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="2">
+        <v>12</v>
+      </c>
+      <c r="G5" s="4">
         <v>30133</v>
       </c>
       <c r="H5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="1" spans="1:8">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="2">
+        <v>12</v>
+      </c>
+      <c r="G6" s="4">
         <v>10000</v>
       </c>
       <c r="H6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" s="1" customFormat="1" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C7"/>
       <c r="D7" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="4">
+        <v>12</v>
+      </c>
+      <c r="G7" s="7">
         <v>2009</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" customFormat="1" spans="1:8">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="2">
+        <v>12</v>
+      </c>
+      <c r="G8" s="4">
         <v>300</v>
       </c>
       <c r="H8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="1" spans="1:8">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="2">
+        <v>12</v>
+      </c>
+      <c r="G9" s="4">
         <v>11000</v>
       </c>
       <c r="H9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" customFormat="1" spans="1:8">
       <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" s="4">
+        <v>72056</v>
+      </c>
+      <c r="H10" t="s">
         <v>38</v>
-      </c>
-      <c r="B10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="2">
-        <v>72056</v>
-      </c>
-      <c r="H10" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="11" customFormat="1" spans="1:8">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="2">
+        <v>12</v>
+      </c>
+      <c r="G11" s="4">
         <v>300</v>
       </c>
       <c r="H11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" customFormat="1" spans="1:8">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="2">
+        <v>12</v>
+      </c>
+      <c r="G12" s="4">
         <v>1999</v>
       </c>
       <c r="H12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" customFormat="1" spans="1:8">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="2">
+        <v>12</v>
+      </c>
+      <c r="G13" s="4">
         <v>7777</v>
       </c>
       <c r="H13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" customFormat="1" spans="1:8">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F14" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="2">
+        <v>12</v>
+      </c>
+      <c r="G14" s="4">
         <v>2500</v>
       </c>
       <c r="H14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" customFormat="1" spans="1:8">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="2">
+        <v>12</v>
+      </c>
+      <c r="G15" s="4">
         <v>8888</v>
       </c>
       <c r="H15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" customFormat="1" spans="1:8">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F16" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" s="2">
+        <v>12</v>
+      </c>
+      <c r="G16" s="4">
         <v>10000</v>
       </c>
       <c r="H16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" customFormat="1" spans="1:8">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F17" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" s="2">
+        <v>12</v>
+      </c>
+      <c r="G17" s="4">
         <v>4444</v>
       </c>
       <c r="H17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" customFormat="1" spans="1:8">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B18" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C18" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F18" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" s="2">
+        <v>12</v>
+      </c>
+      <c r="G18" s="4">
         <v>10000</v>
       </c>
       <c r="H18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" customFormat="1" spans="1:8">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B19" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C19" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F19" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19" s="2">
+        <v>12</v>
+      </c>
+      <c r="G19" s="4">
         <v>10000</v>
       </c>
       <c r="H19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" customFormat="1" spans="1:8">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B20" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C20" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F20" t="s">
-        <v>11</v>
-      </c>
-      <c r="G20" s="2">
+        <v>12</v>
+      </c>
+      <c r="G20" s="4">
         <v>260</v>
       </c>
       <c r="H20" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" customFormat="1" spans="1:8">
       <c r="A21" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B21" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C21" t="s">
-        <v>73</v>
-      </c>
-      <c r="D21" s="3"/>
+        <v>74</v>
+      </c>
+      <c r="D21" s="6"/>
       <c r="F21" t="s">
-        <v>11</v>
-      </c>
-      <c r="G21" s="2">
+        <v>12</v>
+      </c>
+      <c r="G21" s="4">
         <v>54</v>
       </c>
       <c r="H21" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" customFormat="1" spans="1:8">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C22" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F22" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" s="2">
+        <v>12</v>
+      </c>
+      <c r="G22" s="4">
         <v>999</v>
       </c>
       <c r="H22" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" customFormat="1" spans="1:8">
       <c r="A23" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C23" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F23" t="s">
-        <v>11</v>
-      </c>
-      <c r="G23" s="2">
+        <v>12</v>
+      </c>
+      <c r="G23" s="4">
         <v>8888</v>
       </c>
       <c r="H23" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" customFormat="1" spans="1:8">
       <c r="A24" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B24" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C24" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F24" t="s">
-        <v>11</v>
-      </c>
-      <c r="G24" s="2">
+        <v>12</v>
+      </c>
+      <c r="G24" s="4">
         <v>1003</v>
       </c>
       <c r="H24" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" customFormat="1" spans="1:8">
       <c r="A25" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B25" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C25" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F25" t="s">
-        <v>11</v>
-      </c>
-      <c r="G25" s="2">
+        <v>12</v>
+      </c>
+      <c r="G25" s="4">
         <v>700</v>
       </c>
       <c r="H25" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" customFormat="1" spans="1:8">
       <c r="A26" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B26" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C26" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F26" t="s">
-        <v>11</v>
-      </c>
-      <c r="G26" s="2">
+        <v>12</v>
+      </c>
+      <c r="G26" s="4">
         <v>55</v>
       </c>
       <c r="H26" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" customFormat="1" spans="1:8">
       <c r="A27" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B27" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C27" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F27" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" s="2">
+        <v>12</v>
+      </c>
+      <c r="G27" s="4">
         <v>49</v>
       </c>
       <c r="H27" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" customFormat="1" spans="1:8">
       <c r="A28" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B28" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C28" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F28" t="s">
-        <v>11</v>
-      </c>
-      <c r="G28" s="2">
+        <v>12</v>
+      </c>
+      <c r="G28" s="4">
         <v>2222</v>
       </c>
       <c r="H28" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" s="1" customFormat="1" spans="1:8">
       <c r="A29" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C29"/>
       <c r="D29" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G29" s="4">
+        <v>12</v>
+      </c>
+      <c r="G29" s="7">
         <v>2015</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" customFormat="1" spans="1:8">
       <c r="A30" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C30" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F30" t="s">
-        <v>11</v>
-      </c>
-      <c r="G30" s="2">
+        <v>12</v>
+      </c>
+      <c r="G30" s="4">
         <v>102</v>
       </c>
       <c r="H30" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" customFormat="1" spans="1:8">
       <c r="A31" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B31" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C31" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F31" t="s">
-        <v>11</v>
-      </c>
-      <c r="G31" s="2">
+        <v>12</v>
+      </c>
+      <c r="G31" s="4">
         <v>10000</v>
       </c>
       <c r="H31" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" customFormat="1" spans="1:8">
       <c r="A32" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B32" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C32" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F32" t="s">
-        <v>11</v>
-      </c>
-      <c r="G32" s="2">
+        <v>12</v>
+      </c>
+      <c r="G32" s="4">
         <v>137</v>
       </c>
       <c r="H32" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" customFormat="1" spans="1:8">
       <c r="A33" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B33" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C33" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F33" t="s">
-        <v>11</v>
-      </c>
-      <c r="G33" s="2">
+        <v>12</v>
+      </c>
+      <c r="G33" s="4">
         <v>50</v>
       </c>
       <c r="H33" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" customFormat="1" spans="1:8">
       <c r="A34" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B34" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C34" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F34" t="s">
-        <v>11</v>
-      </c>
-      <c r="G34" s="2">
+        <v>12</v>
+      </c>
+      <c r="G34" s="4">
         <v>300</v>
       </c>
       <c r="H34" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35" customFormat="1" spans="1:8">
       <c r="A35" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B35" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C35" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F35" t="s">
-        <v>11</v>
-      </c>
-      <c r="G35" s="2">
+        <v>12</v>
+      </c>
+      <c r="G35" s="4">
         <v>3333</v>
       </c>
       <c r="H35" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" customFormat="1" spans="1:8">
       <c r="A36" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B36" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C36" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F36" t="s">
-        <v>11</v>
-      </c>
-      <c r="G36" s="2">
+        <v>12</v>
+      </c>
+      <c r="G36" s="4">
         <v>4444</v>
       </c>
       <c r="H36" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" customFormat="1" spans="1:8">
       <c r="A37" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B37" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C37" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F37" t="s">
-        <v>11</v>
-      </c>
-      <c r="G37" s="2">
+        <v>12</v>
+      </c>
+      <c r="G37" s="4">
         <v>8888</v>
       </c>
       <c r="H37" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" customFormat="1" spans="1:8">
       <c r="A38" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B38" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C38" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F38" t="s">
-        <v>11</v>
-      </c>
-      <c r="G38" s="2">
+        <v>12</v>
+      </c>
+      <c r="G38" s="4">
         <v>8888</v>
       </c>
       <c r="H38" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" customFormat="1" spans="1:8">
       <c r="A39" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B39" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C39" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F39" t="s">
-        <v>127</v>
-      </c>
-      <c r="G39" s="2">
+        <v>128</v>
+      </c>
+      <c r="G39" s="4">
         <v>8001</v>
       </c>
-      <c r="H39" s="5" t="s">
-        <v>37</v>
+      <c r="H39" s="8" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="40" customFormat="1" spans="1:8">
       <c r="A40" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B40" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C40" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F40" t="s">
-        <v>11</v>
-      </c>
-      <c r="G40" s="2">
+        <v>12</v>
+      </c>
+      <c r="G40" s="4">
         <v>10000</v>
       </c>
       <c r="H40" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" customFormat="1" spans="1:8">
       <c r="A41" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B41" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C41" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F41" t="s">
-        <v>11</v>
-      </c>
-      <c r="G41" s="2">
+        <v>12</v>
+      </c>
+      <c r="G41" s="4">
         <v>2222</v>
       </c>
       <c r="H41" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42" customFormat="1" spans="1:8">
       <c r="A42" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B42" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C42" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F42" t="s">
-        <v>11</v>
-      </c>
-      <c r="G42" s="2">
+        <v>12</v>
+      </c>
+      <c r="G42" s="4">
         <v>1500</v>
       </c>
       <c r="H42" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" customFormat="1" spans="1:8">
       <c r="A43" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B43" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C43" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F43" t="s">
-        <v>11</v>
-      </c>
-      <c r="G43" s="2">
+        <v>12</v>
+      </c>
+      <c r="G43" s="4">
         <v>100</v>
       </c>
       <c r="H43" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" customFormat="1" spans="1:8">
       <c r="A44" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B44" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C44" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F44" t="s">
-        <v>11</v>
-      </c>
-      <c r="G44" s="2">
+        <v>12</v>
+      </c>
+      <c r="G44" s="4">
         <v>8888</v>
       </c>
       <c r="H44" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45" customFormat="1" spans="1:8">
       <c r="A45" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B45" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C45" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F45" t="s">
-        <v>11</v>
-      </c>
-      <c r="G45" s="2">
+        <v>12</v>
+      </c>
+      <c r="G45" s="4">
         <v>9788</v>
       </c>
       <c r="H45" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46" customFormat="1" spans="1:8">
       <c r="A46" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B46" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C46" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F46" t="s">
-        <v>11</v>
-      </c>
-      <c r="G46" s="2">
+        <v>12</v>
+      </c>
+      <c r="G46" s="4">
         <v>10000</v>
       </c>
       <c r="H46" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="47" customFormat="1" spans="1:8">
       <c r="A47" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B47" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C47" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F47" t="s">
-        <v>127</v>
-      </c>
-      <c r="G47" s="2">
+        <v>128</v>
+      </c>
+      <c r="G47" s="4">
         <v>10000</v>
       </c>
       <c r="H47" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="48" customFormat="1" spans="1:8">
       <c r="A48" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B48" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C48" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F48" t="s">
-        <v>11</v>
-      </c>
-      <c r="G48" s="2">
+        <v>12</v>
+      </c>
+      <c r="G48" s="4">
         <v>99</v>
       </c>
       <c r="H48" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="49" customFormat="1" spans="1:8">
       <c r="A49" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B49" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C49" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F49" t="s">
-        <v>11</v>
-      </c>
-      <c r="G49" s="2">
+        <v>12</v>
+      </c>
+      <c r="G49" s="4">
         <v>60000</v>
       </c>
       <c r="H49" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="50" customFormat="1" spans="1:8">
       <c r="A50" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B50" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C50" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F50" t="s">
-        <v>11</v>
-      </c>
-      <c r="G50" s="2">
+        <v>12</v>
+      </c>
+      <c r="G50" s="4">
         <v>10000</v>
       </c>
       <c r="H50" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="51" customFormat="1" spans="1:8">
       <c r="A51" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B51" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C51" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F51" t="s">
-        <v>11</v>
-      </c>
-      <c r="G51" s="2">
+        <v>12</v>
+      </c>
+      <c r="G51" s="4">
         <v>2222</v>
       </c>
       <c r="H51" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="52" customFormat="1" spans="1:8">
       <c r="A52" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B52" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C52" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F52" t="s">
-        <v>11</v>
-      </c>
-      <c r="G52" s="2">
+        <v>12</v>
+      </c>
+      <c r="G52" s="4">
         <v>10000</v>
       </c>
       <c r="H52" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="53" customFormat="1" spans="1:8">
       <c r="A53" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B53" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C53" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F53" t="s">
-        <v>11</v>
-      </c>
-      <c r="G53" s="2">
+        <v>12</v>
+      </c>
+      <c r="G53" s="4">
         <v>5555</v>
       </c>
       <c r="H53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="54" customFormat="1" spans="1:8">
       <c r="A54" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B54" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C54" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F54" t="s">
-        <v>11</v>
-      </c>
-      <c r="G54" s="2">
+        <v>12</v>
+      </c>
+      <c r="G54" s="4">
         <v>10000</v>
       </c>
       <c r="H54" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="55" customFormat="1" spans="1:8">
       <c r="A55" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B55" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C55" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F55" t="s">
-        <v>11</v>
-      </c>
-      <c r="G55" s="2">
+        <v>12</v>
+      </c>
+      <c r="G55" s="4">
         <v>3001</v>
       </c>
       <c r="H55" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56" customFormat="1" spans="1:8">
       <c r="A56" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B56" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C56" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F56" t="s">
-        <v>11</v>
-      </c>
-      <c r="G56" s="2">
+        <v>12</v>
+      </c>
+      <c r="G56" s="4">
         <v>10000</v>
       </c>
       <c r="H56" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="57" customFormat="1" spans="1:8">
       <c r="A57" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B57" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C57" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F57" t="s">
-        <v>11</v>
-      </c>
-      <c r="G57" s="2">
+        <v>12</v>
+      </c>
+      <c r="G57" s="4">
         <v>500</v>
       </c>
       <c r="H57" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="58" customFormat="1" spans="1:8">
       <c r="A58" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B58" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C58" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F58" t="s">
-        <v>11</v>
-      </c>
-      <c r="G58" s="2">
+        <v>12</v>
+      </c>
+      <c r="G58" s="4">
         <v>10</v>
       </c>
       <c r="H58" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="59" customFormat="1" spans="1:8">
       <c r="A59" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B59" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C59" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F59" t="s">
-        <v>11</v>
-      </c>
-      <c r="G59" s="2">
+        <v>12</v>
+      </c>
+      <c r="G59" s="4">
         <v>6598</v>
       </c>
       <c r="H59" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="60" customFormat="1" spans="1:8">
       <c r="A60" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B60" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C60" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F60" t="s">
-        <v>11</v>
-      </c>
-      <c r="G60" s="2">
+        <v>12</v>
+      </c>
+      <c r="G60" s="4">
         <v>9999</v>
       </c>
       <c r="H60" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="61" customFormat="1" spans="1:8">
       <c r="A61" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B61" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C61" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F61" t="s">
-        <v>127</v>
-      </c>
-      <c r="G61" s="2">
+        <v>128</v>
+      </c>
+      <c r="G61" s="4">
         <v>10000</v>
       </c>
       <c r="H61" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="62" customFormat="1" spans="1:8">
       <c r="A62" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B62" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C62" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F62" t="s">
-        <v>11</v>
-      </c>
-      <c r="G62" s="2">
+        <v>12</v>
+      </c>
+      <c r="G62" s="4">
         <v>7777</v>
       </c>
       <c r="H62" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="63" customFormat="1" spans="1:8">
       <c r="A63" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B63" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C63" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F63" t="s">
-        <v>11</v>
-      </c>
-      <c r="G63" s="2">
+        <v>12</v>
+      </c>
+      <c r="G63" s="4">
         <v>11111</v>
       </c>
       <c r="H63" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="64" customFormat="1" spans="1:8">
       <c r="A64" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B64" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C64" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F64" t="s">
-        <v>11</v>
-      </c>
-      <c r="G64" s="2">
+        <v>12</v>
+      </c>
+      <c r="G64" s="4">
         <v>1000</v>
       </c>
       <c r="H64" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="65" customFormat="1" spans="1:8">
       <c r="A65" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B65" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C65" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F65" t="s">
-        <v>11</v>
-      </c>
-      <c r="G65" s="2">
+        <v>12</v>
+      </c>
+      <c r="G65" s="4">
         <v>4000</v>
       </c>
       <c r="H65" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="66" customFormat="1" spans="1:8">
       <c r="A66" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B66" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C66" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F66" t="s">
-        <v>127</v>
-      </c>
-      <c r="G66" s="2">
+        <v>128</v>
+      </c>
+      <c r="G66" s="4">
         <v>10000</v>
       </c>
       <c r="H66" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="67" customFormat="1" spans="1:8">
       <c r="A67" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B67" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C67" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F67" t="s">
-        <v>11</v>
-      </c>
-      <c r="G67" s="2">
+        <v>12</v>
+      </c>
+      <c r="G67" s="4">
         <v>10000</v>
       </c>
       <c r="H67" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="68" customFormat="1" spans="1:8">
       <c r="A68" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B68" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C68" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F68" t="s">
-        <v>11</v>
-      </c>
-      <c r="G68" s="2">
+        <v>12</v>
+      </c>
+      <c r="G68" s="4">
         <v>2878</v>
       </c>
       <c r="H68" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="69" customFormat="1" spans="1:8">
       <c r="A69" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B69" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C69" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="F69" t="s">
-        <v>11</v>
-      </c>
-      <c r="G69" s="2">
+        <v>12</v>
+      </c>
+      <c r="G69" s="4">
         <v>3534</v>
       </c>
       <c r="H69" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="70" customFormat="1" spans="1:8">
       <c r="A70" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B70" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C70" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F70" t="s">
-        <v>11</v>
-      </c>
-      <c r="G70" s="2">
+        <v>12</v>
+      </c>
+      <c r="G70" s="4">
         <v>10000</v>
       </c>
       <c r="H70" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="71" customFormat="1" spans="1:8">
       <c r="A71" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B71" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C71" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="F71" t="s">
-        <v>11</v>
-      </c>
-      <c r="G71" s="2">
+        <v>12</v>
+      </c>
+      <c r="G71" s="4">
         <v>9999</v>
       </c>
       <c r="H71" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="72" customFormat="1" spans="1:8">
       <c r="A72" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C72" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
-      <c r="G72" s="4">
+      <c r="G72" s="7">
         <v>10000</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="73" customFormat="1" spans="1:8">
       <c r="A73" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B73" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C73" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F73" t="s">
-        <v>11</v>
-      </c>
-      <c r="G73" s="2">
+        <v>12</v>
+      </c>
+      <c r="G73" s="4">
         <v>10000</v>
       </c>
       <c r="H73" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="74" customFormat="1" spans="1:8">
       <c r="A74" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B74" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C74" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F74" t="s">
-        <v>11</v>
-      </c>
-      <c r="G74" s="2">
+        <v>12</v>
+      </c>
+      <c r="G74" s="4">
         <v>5555</v>
       </c>
       <c r="H74" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="75" customFormat="1" spans="1:8">
       <c r="A75" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B75" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C75" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F75" t="s">
-        <v>11</v>
-      </c>
-      <c r="G75" s="2">
+        <v>12</v>
+      </c>
+      <c r="G75" s="4">
         <v>160</v>
       </c>
       <c r="H75" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="76" customFormat="1" spans="1:8">
       <c r="A76" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B76" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C76" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F76" t="s">
-        <v>11</v>
-      </c>
-      <c r="G76" s="2">
+        <v>12</v>
+      </c>
+      <c r="G76" s="4">
         <v>666</v>
       </c>
       <c r="H76" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="77" customFormat="1" spans="1:8">
       <c r="A77" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B77" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C77" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F77" t="s">
-        <v>11</v>
-      </c>
-      <c r="G77" s="2">
+        <v>12</v>
+      </c>
+      <c r="G77" s="4">
         <v>6000</v>
       </c>
       <c r="H77" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="78" customFormat="1" spans="1:8">
       <c r="A78" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B78" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C78" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F78" t="s">
-        <v>11</v>
-      </c>
-      <c r="G78" s="2">
+        <v>12</v>
+      </c>
+      <c r="G78" s="4">
         <v>170</v>
       </c>
       <c r="H78" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="79" customFormat="1" spans="1:8">
       <c r="A79" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B79" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C79" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F79" t="s">
-        <v>11</v>
-      </c>
-      <c r="G79" s="2">
+        <v>12</v>
+      </c>
+      <c r="G79" s="4">
         <v>10000</v>
       </c>
       <c r="H79" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="80" customFormat="1" spans="1:8">
       <c r="A80" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B80" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C80" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="F80" t="s">
-        <v>11</v>
-      </c>
-      <c r="G80" s="2">
+        <v>12</v>
+      </c>
+      <c r="G80" s="4">
         <v>222</v>
       </c>
       <c r="H80" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="81" customFormat="1" spans="1:8">
       <c r="A81" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B81" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C81" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F81" t="s">
-        <v>11</v>
-      </c>
-      <c r="G81" s="2">
+        <v>12</v>
+      </c>
+      <c r="G81" s="4">
         <v>10000</v>
       </c>
       <c r="H81" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="82" customFormat="1" spans="1:8">
       <c r="A82" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B82" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C82" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F82" t="s">
-        <v>11</v>
-      </c>
-      <c r="G82" s="2">
+        <v>12</v>
+      </c>
+      <c r="G82" s="4">
         <v>2000</v>
       </c>
       <c r="H82" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="83" customFormat="1" spans="1:8">
       <c r="A83" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B83" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C83" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F83" t="s">
-        <v>11</v>
-      </c>
-      <c r="G83" s="2">
+        <v>12</v>
+      </c>
+      <c r="G83" s="4">
         <v>7777</v>
       </c>
       <c r="H83" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="84" customFormat="1" spans="1:8">
       <c r="A84" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B84" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C84" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="F84" t="s">
-        <v>11</v>
-      </c>
-      <c r="G84" s="2">
+        <v>12</v>
+      </c>
+      <c r="G84" s="4">
         <v>9976</v>
       </c>
       <c r="H84" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="85" customFormat="1" spans="1:8">
       <c r="A85" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B85" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C85" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="F85" t="s">
-        <v>11</v>
-      </c>
-      <c r="G85" s="2">
+        <v>12</v>
+      </c>
+      <c r="G85" s="4">
         <v>10000</v>
       </c>
       <c r="H85" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="86" customFormat="1" spans="1:8">
       <c r="A86" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B86" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C86" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="F86" t="s">
-        <v>11</v>
-      </c>
-      <c r="G86" s="2">
+        <v>12</v>
+      </c>
+      <c r="G86" s="4">
         <v>3</v>
       </c>
       <c r="H86" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="87" customFormat="1" spans="1:8">
       <c r="A87" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B87" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C87" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="F87" t="s">
-        <v>11</v>
-      </c>
-      <c r="G87" s="2">
+        <v>12</v>
+      </c>
+      <c r="G87" s="4">
         <v>7777</v>
       </c>
       <c r="H87" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="88" customFormat="1" spans="1:8">
       <c r="A88" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B88" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C88" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="F88" t="s">
-        <v>11</v>
-      </c>
-      <c r="G88" s="2">
+        <v>12</v>
+      </c>
+      <c r="G88" s="4">
         <v>1000</v>
       </c>
       <c r="H88" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="89" customFormat="1" spans="1:8">
       <c r="A89" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B89" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C89" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F89" t="s">
-        <v>11</v>
-      </c>
-      <c r="G89" s="2">
+        <v>12</v>
+      </c>
+      <c r="G89" s="4">
         <v>81</v>
       </c>
       <c r="H89" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="90" customFormat="1" spans="1:8">
       <c r="A90" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B90" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C90" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="F90" t="s">
-        <v>11</v>
-      </c>
-      <c r="G90" s="2">
+        <v>12</v>
+      </c>
+      <c r="G90" s="4">
         <v>9999</v>
       </c>
       <c r="H90" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="91" customFormat="1" spans="1:8">
       <c r="A91" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B91" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C91" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="F91" t="s">
-        <v>11</v>
-      </c>
-      <c r="G91" s="2">
+        <v>12</v>
+      </c>
+      <c r="G91" s="4">
         <v>50</v>
       </c>
       <c r="H91" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="92" customFormat="1" spans="1:8">
       <c r="A92" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B92" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C92" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="F92" t="s">
-        <v>11</v>
-      </c>
-      <c r="G92" s="2">
+        <v>12</v>
+      </c>
+      <c r="G92" s="4">
         <v>10000</v>
       </c>
       <c r="H92" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="93" customFormat="1" spans="1:8">
       <c r="A93" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B93" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C93" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="F93" t="s">
-        <v>11</v>
-      </c>
-      <c r="G93" s="2">
+        <v>12</v>
+      </c>
+      <c r="G93" s="4">
         <v>10000</v>
       </c>
       <c r="H93" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="94" customFormat="1" spans="1:8">
       <c r="A94" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B94" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C94" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="F94" t="s">
-        <v>11</v>
-      </c>
-      <c r="G94" s="2">
+        <v>12</v>
+      </c>
+      <c r="G94" s="4">
         <v>888</v>
       </c>
       <c r="H94" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="95" customFormat="1" spans="1:8">
       <c r="A95" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B95" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C95" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="F95" t="s">
-        <v>11</v>
-      </c>
-      <c r="G95" s="2">
+        <v>12</v>
+      </c>
+      <c r="G95" s="4">
         <v>117</v>
       </c>
       <c r="H95" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="96" customFormat="1" spans="1:8">
       <c r="A96" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B96" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C96" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="F96" t="s">
-        <v>11</v>
-      </c>
-      <c r="G96" s="2">
+        <v>12</v>
+      </c>
+      <c r="G96" s="4">
         <v>2</v>
       </c>
       <c r="H96" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="97" customFormat="1" spans="1:8">
       <c r="A97" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B97" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C97" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="F97" t="s">
-        <v>11</v>
-      </c>
-      <c r="G97" s="2">
+        <v>12</v>
+      </c>
+      <c r="G97" s="4">
         <v>3</v>
       </c>
       <c r="H97" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="98" customFormat="1" spans="1:8">
       <c r="A98" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B98" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C98" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F98" t="s">
-        <v>11</v>
-      </c>
-      <c r="G98" s="2">
+        <v>12</v>
+      </c>
+      <c r="G98" s="4">
         <v>5500</v>
       </c>
       <c r="H98" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="99" customFormat="1" spans="1:8">
       <c r="A99" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B99" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C99" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="F99" t="s">
-        <v>11</v>
-      </c>
-      <c r="G99" s="2">
+        <v>12</v>
+      </c>
+      <c r="G99" s="4">
         <v>10000</v>
       </c>
       <c r="H99" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="100" customFormat="1" spans="1:8">
       <c r="A100" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B100" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C100" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="F100" t="s">
-        <v>11</v>
-      </c>
-      <c r="G100" s="2">
+        <v>12</v>
+      </c>
+      <c r="G100" s="4">
         <v>110</v>
       </c>
       <c r="H100" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="101" customFormat="1" spans="1:8">
       <c r="A101" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B101" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C101" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="F101" t="s">
-        <v>11</v>
-      </c>
-      <c r="G101" s="2">
+        <v>12</v>
+      </c>
+      <c r="G101" s="4">
         <v>10000</v>
       </c>
       <c r="H101" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="102" customFormat="1" spans="1:8">
       <c r="A102" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B102" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C102" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="F102" t="s">
-        <v>11</v>
-      </c>
-      <c r="G102" s="2">
+        <v>12</v>
+      </c>
+      <c r="G102" s="4">
         <v>99</v>
       </c>
       <c r="H102" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="103" customFormat="1" spans="1:8">
       <c r="A103" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B103" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C103" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="F103" t="s">
-        <v>11</v>
-      </c>
-      <c r="G103" s="2">
+        <v>12</v>
+      </c>
+      <c r="G103" s="4">
         <v>5555</v>
       </c>
       <c r="H103" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="104" customFormat="1" spans="1:8">
       <c r="A104" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B104" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C104" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="F104" t="s">
-        <v>11</v>
-      </c>
-      <c r="G104" s="2">
+        <v>12</v>
+      </c>
+      <c r="G104" s="4">
         <v>2</v>
       </c>
       <c r="H104" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="105" customFormat="1" spans="1:8">
       <c r="A105" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B105" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C105" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="F105" t="s">
-        <v>11</v>
-      </c>
-      <c r="G105" s="2">
+        <v>12</v>
+      </c>
+      <c r="G105" s="4">
         <v>5000</v>
       </c>
       <c r="H105" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="106" customFormat="1" spans="1:8">
       <c r="A106" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B106" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C106" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="F106" t="s">
-        <v>11</v>
-      </c>
-      <c r="G106" s="2">
+        <v>12</v>
+      </c>
+      <c r="G106" s="4">
         <v>420</v>
       </c>
       <c r="H106" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="107" customFormat="1" spans="1:8">
       <c r="A107" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B107" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C107" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="F107" t="s">
-        <v>11</v>
-      </c>
-      <c r="G107" s="2">
+        <v>12</v>
+      </c>
+      <c r="G107" s="4">
         <v>2880</v>
       </c>
       <c r="H107" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="108" customFormat="1" spans="1:8">
       <c r="A108" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B108" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C108" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="F108" t="s">
-        <v>11</v>
-      </c>
-      <c r="G108" s="2">
+        <v>12</v>
+      </c>
+      <c r="G108" s="4">
         <v>500</v>
       </c>
       <c r="H108" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="109" customFormat="1" spans="1:8">
       <c r="A109" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B109" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C109" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="F109" t="s">
-        <v>11</v>
-      </c>
-      <c r="G109" s="2">
+        <v>12</v>
+      </c>
+      <c r="G109" s="4">
         <v>87</v>
       </c>
       <c r="H109" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="110" customFormat="1" spans="1:8">
       <c r="A110" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B110" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C110" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="F110" t="s">
-        <v>11</v>
-      </c>
-      <c r="G110" s="2">
+        <v>12</v>
+      </c>
+      <c r="G110" s="4">
         <v>8888</v>
       </c>
       <c r="H110" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="111" s="2" customFormat="1" spans="1:9">
+      <c r="A111" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="B111" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="C111" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="D111" s="9"/>
+      <c r="E111" s="9"/>
+      <c r="F111" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G111" s="9">
+        <v>3996</v>
+      </c>
+      <c r="H111" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I111" s="9" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="112" s="3" customFormat="1" ht="23" customHeight="1" spans="1:9">
+      <c r="A112" s="9" t="s">
+        <v>345</v>
+      </c>
+      <c r="B112" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="C112" s="9" t="s">
+        <v>347</v>
+      </c>
+      <c r="D112" s="9"/>
+      <c r="E112" s="9"/>
+      <c r="F112" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G112" s="9">
+        <v>6666</v>
+      </c>
+      <c r="H112" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="I112" s="9" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="113" s="3" customFormat="1" spans="1:9">
+      <c r="A113" s="9" t="s">
+        <v>349</v>
+      </c>
+      <c r="B113" s="9" t="s">
+        <v>350</v>
+      </c>
+      <c r="C113" s="9" t="s">
+        <v>351</v>
+      </c>
+      <c r="D113" s="9"/>
+      <c r="E113" s="9"/>
+      <c r="F113" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G113" s="9">
+        <v>176</v>
+      </c>
+      <c r="H113" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I113" s="9" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="114" s="3" customFormat="1" spans="1:9">
+      <c r="A114" s="9" t="s">
+        <v>352</v>
+      </c>
+      <c r="B114" s="9" t="s">
+        <v>353</v>
+      </c>
+      <c r="C114" s="9" t="s">
+        <v>354</v>
+      </c>
+      <c r="D114" s="9"/>
+      <c r="E114" s="9"/>
+      <c r="F114" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G114" s="9">
+        <v>3969</v>
+      </c>
+      <c r="H114" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="I114" s="9" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="115" s="3" customFormat="1" spans="1:9">
+      <c r="A115" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="B115" s="9" t="s">
+        <v>356</v>
+      </c>
+      <c r="C115" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="D115" s="9"/>
+      <c r="E115" s="9"/>
+      <c r="F115" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G115" s="9">
+        <v>999</v>
+      </c>
+      <c r="H115" s="9" t="s">
+        <v>358</v>
+      </c>
+      <c r="I115" s="9" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="116" s="3" customFormat="1" spans="1:9">
+      <c r="A116" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="B116" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="C116" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="D116" s="9"/>
+      <c r="E116" s="9"/>
+      <c r="F116" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G116" s="9">
+        <v>7777</v>
+      </c>
+      <c r="H116" s="9" t="s">
+        <v>358</v>
+      </c>
+      <c r="I116" s="9" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="117" s="3" customFormat="1" spans="1:9">
+      <c r="A117" s="9" t="s">
+        <v>362</v>
+      </c>
+      <c r="B117" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="C117" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="D117" s="9"/>
+      <c r="E117" s="9"/>
+      <c r="F117" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G117" s="9">
+        <v>10000</v>
+      </c>
+      <c r="H117" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="I117" s="9" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="118" s="3" customFormat="1" spans="1:9">
+      <c r="A118" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="B118" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="C118" s="9" t="s">
+        <v>367</v>
+      </c>
+      <c r="D118" s="9"/>
+      <c r="E118" s="9"/>
+      <c r="F118" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G118" s="9">
+        <v>5684</v>
+      </c>
+      <c r="H118" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I118" s="9" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="149" ht="20" spans="14:14">
-      <c r="N149" s="6" t="s">
-        <v>341</v>
+      <c r="N149" s="10" t="s">
+        <v>368</v>
       </c>
     </row>
   </sheetData>
@@ -4277,7 +4581,15 @@
     <hyperlink ref="C61" r:id="rId15" display="https://fp7fo-2aaaa-aaaaf-qaeea-cai.raw.ic0.app/Token/%d" tooltip="https://fp7fo-2aaaa-aaaaf-qaeea-cai.raw.ic0.app/Token/%d"/>
     <hyperlink ref="C38" r:id="rId16" display="https://yrdz3-2yaaa-aaaah-qcvpa-cai.raw.ic0.app/?type=thumbnail&amp;tokenid=%s" tooltip="https://yrdz3-2yaaa-aaaah-qcvpa-cai.raw.ic0.app/?type=thumbnail&amp;tokenid=%s"/>
     <hyperlink ref="C59" r:id="rId17" display="https://po6n2-uiaaa-aaaaj-qaiua-cai.raw.ic0.app/?tokenid=%s"/>
-    <hyperlink ref="C67" r:id="rId18" display="https://njgly-uaaaa-aaaah-qb6pa-cai.raw.ic0.app/?type=thumbnail&amp;tokenid=%s"/>
+    <hyperlink ref="C112" r:id="rId18" display="https://2tvxo-eqaaa-aaaai-acjla-cai.raw.ic0.app/?type=thumbnail&amp;tokenid=%s"/>
+    <hyperlink ref="C113" r:id="rId19" display="https://x4oqm-bqaaa-aaaam-qahaq-cai.raw.ic0.app/?type=thumbnail&amp;tokenid=%s" tooltip="https://x4oqm-bqaaa-aaaam-qahaq-cai.raw.ic0.app/?type=thumbnail&amp;tokenid=%s"/>
+    <hyperlink ref="C114" r:id="rId20" display="https://y5prr-fiaaa-aaaam-qagga-cai.raw.ic0.app/?type=thumbnail&amp;tokenid=%s" tooltip="https://y5prr-fiaaa-aaaam-qagga-cai.raw.ic0.app/?type=thumbnail&amp;tokenid=%s"/>
+    <hyperlink ref="C115" r:id="rId21" display="https://6wghg-7yaaa-aaaam-qagra-cai.raw.ic0.app/?type=thumbnail&amp;tokenid=%s" tooltip="https://6wghg-7yaaa-aaaam-qagra-cai.raw.ic0.app/?type=thumbnail&amp;tokenid=%s"/>
+    <hyperlink ref="C116" r:id="rId22" display="https://6eaq7-tiaaa-aaaam-qagsa-cai.raw.ic0.app/?type=thumbnail&amp;tokenid=%s"/>
+    <hyperlink ref="C117" r:id="rId23" display="https://vcpye-qyaaa-aaaak-qafjq-cai.raw.ic0.app/?type=thumbnail&amp;tokenid=%s"/>
+    <hyperlink ref="C118" r:id="rId24" display="https://tvo7m-iyaaa-aaaai-qjjsa-cai.raw.ic0.app/?type=thumbnail&amp;tokenid=%s"/>
+    <hyperlink ref="C67" r:id="rId25" display="https://njgly-uaaaa-aaaah-qb6pa-cai.raw.ic0.app/?type=thumbnail&amp;tokenid=%s"/>
+    <hyperlink ref="C111" r:id="rId26" display="https://jmuqr-yqaaa-aaaaj-qaicq-cai.raw.ic0.app/?type=thumbnail&amp;tokenid=%s" tooltip="https://jmuqr-yqaaa-aaaaj-qaicq-cai.raw.ic0.app/?type=thumbnail&amp;tokenid=%s"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>